<commit_message>
Incorporate Manual Override Dictionary
Defined a dictionary that maps known problematic school names to their correct counterparts. Still does not work.
</commit_message>
<xml_diff>
--- a/Updated Zone 1 Activity Playground.xlsx
+++ b/Updated Zone 1 Activity Playground.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A99CD2-E830-5643-B6DE-6DA550E64DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1426" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="822">
   <si>
     <t>Member/Non-Member - Organization</t>
   </si>
@@ -2421,16 +2427,22 @@
     <t>2016; 2023</t>
   </si>
   <si>
+    <t>2023; 2024</t>
+  </si>
+  <si>
+    <t>2022; 2023; 2024</t>
+  </si>
+  <si>
+    <t>2016; 2017; 2018; 2019; 2021; 2022; 2023; 2024</t>
+  </si>
+  <si>
     <t>2022; 2023</t>
   </si>
   <si>
-    <t>2016; 2017; 2018; 2019; 2021; 2022; 2023</t>
-  </si>
-  <si>
-    <t>2015; 2016; 2017; 2018; 2019; 2021; 2023</t>
-  </si>
-  <si>
-    <t>2015; 2016; 2017; 2018; 2019; 2021; 2022; 2023</t>
+    <t>2015; 2016; 2017; 2018; 2019; 2021; 2023; 2024</t>
+  </si>
+  <si>
+    <t>2015; 2016; 2017; 2018; 2019; 2021; 2022; 2023; 2024</t>
   </si>
   <si>
     <t>2021; 2023</t>
@@ -2439,10 +2451,10 @@
     <t>2017; 2018; 2019; 2021; 2022; 2023</t>
   </si>
   <si>
-    <t>2021; 2022; 2023</t>
-  </si>
-  <si>
-    <t>2018; 2019; 2022; 2023</t>
+    <t>2021; 2022; 2023; 2024</t>
+  </si>
+  <si>
+    <t>2018; 2019; 2022; 2023; 2024</t>
   </si>
   <si>
     <t>2015; 2016; 2017; 2018; 2021</t>
@@ -2451,16 +2463,22 @@
     <t>2019; 2021</t>
   </si>
   <si>
+    <t>2015; 2016; 2017; 2018; 2019; 2021; 2024</t>
+  </si>
+  <si>
+    <t>2016; 2017; 2018; 2019; 2021; 2024</t>
+  </si>
+  <si>
     <t>2015; 2016; 2017; 2018; 2019; 2021</t>
   </si>
   <si>
-    <t>2016; 2017; 2018; 2019; 2021</t>
-  </si>
-  <si>
     <t>2015; 2017</t>
   </si>
   <si>
     <t>2015; 2016; 2018; 2019; 2021</t>
+  </si>
+  <si>
+    <t>2024</t>
   </si>
   <si>
     <t>2017; 2018; 2019; 2021</t>
@@ -2484,11 +2502,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2552,13 +2570,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2596,7 +2622,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2630,6 +2656,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2664,9 +2691,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2839,14 +2867,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="W34" sqref="W34"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="16" max="16" width="34.1640625" customWidth="1"/>
+    <col min="17" max="17" width="31.1640625" customWidth="1"/>
+    <col min="22" max="22" width="39" customWidth="1"/>
+    <col min="23" max="23" width="68.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3001,7 +3037,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3117,7 +3153,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -3218,7 +3254,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3301,7 +3337,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -3389,11 +3425,11 @@
       <c r="AX5" t="s">
         <v>775</v>
       </c>
-      <c r="AY5">
-        <v>2023</v>
+      <c r="AY5" t="s">
+        <v>798</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -3482,7 +3518,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3603,11 +3639,11 @@
       <c r="AX7" t="s">
         <v>777</v>
       </c>
-      <c r="AY7">
-        <v>2023</v>
+      <c r="AY7" t="s">
+        <v>798</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -3722,11 +3758,11 @@
       <c r="AS8" t="s">
         <v>761</v>
       </c>
-      <c r="AY8">
-        <v>2023</v>
+      <c r="AY8" t="s">
+        <v>798</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -3824,10 +3860,10 @@
         <v>778</v>
       </c>
       <c r="AY9" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -3931,7 +3967,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -4023,10 +4059,10 @@
         <v>779</v>
       </c>
       <c r="AY11" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -4130,10 +4166,10 @@
         <v>780</v>
       </c>
       <c r="AY12" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -4228,10 +4264,10 @@
         <v>775</v>
       </c>
       <c r="AY13" t="s">
-        <v>798</v>
+        <v>801</v>
       </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4347,10 +4383,10 @@
         <v>781</v>
       </c>
       <c r="AY14" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4481,10 +4517,10 @@
         <v>775</v>
       </c>
       <c r="AY15" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
     </row>
-    <row r="16" spans="1:51">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4570,10 +4606,10 @@
         <v>766</v>
       </c>
       <c r="AY16" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
-    <row r="17" spans="1:51">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -4686,7 +4722,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="18" spans="1:51">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -4781,7 +4817,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="19" spans="1:51">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -4894,10 +4930,10 @@
         <v>783</v>
       </c>
       <c r="AY19" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
     </row>
-    <row r="20" spans="1:51">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -5010,10 +5046,10 @@
         <v>775</v>
       </c>
       <c r="AY20" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
     </row>
-    <row r="21" spans="1:51">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -5117,10 +5153,10 @@
         <v>784</v>
       </c>
       <c r="AY21" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
     </row>
-    <row r="22" spans="1:51">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -5176,7 +5212,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="23" spans="1:51">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -5289,7 +5325,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="24" spans="1:51">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -5375,10 +5411,10 @@
         <v>2019</v>
       </c>
       <c r="AY24" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
     </row>
-    <row r="25" spans="1:51">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -5482,10 +5518,10 @@
         <v>2012</v>
       </c>
       <c r="AY25" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
     </row>
-    <row r="26" spans="1:51">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -5577,7 +5613,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="27" spans="1:51">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -5678,10 +5714,10 @@
         <v>775</v>
       </c>
       <c r="AY27" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
     </row>
-    <row r="28" spans="1:51">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -5758,10 +5794,10 @@
         <v>77</v>
       </c>
       <c r="AY28" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
     </row>
-    <row r="29" spans="1:51">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -5856,7 +5892,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="30" spans="1:51">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -5888,7 +5924,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="31" spans="1:51">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -5920,7 +5956,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="32" spans="1:51">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -5982,7 +6018,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="33" spans="1:51">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -6008,7 +6044,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:51">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -6046,7 +6082,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="35" spans="1:51">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -6120,7 +6156,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="36" spans="1:51">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -6191,7 +6227,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="37" spans="1:51">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -6220,7 +6256,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="38" spans="1:51">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -6312,7 +6348,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="39" spans="1:51">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -6401,7 +6437,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="40" spans="1:51">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -6475,10 +6511,10 @@
         <v>775</v>
       </c>
       <c r="AY40" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
-    <row r="41" spans="1:51">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -6567,7 +6603,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="42" spans="1:51">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -6656,7 +6692,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="43" spans="1:51">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -6727,7 +6763,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="44" spans="1:51">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -6756,7 +6792,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:51">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -6788,7 +6824,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:51">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -6817,10 +6853,10 @@
         <v>95</v>
       </c>
       <c r="AY46" t="s">
-        <v>810</v>
+        <v>813</v>
       </c>
     </row>
-    <row r="47" spans="1:51">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -6912,10 +6948,10 @@
         <v>788</v>
       </c>
       <c r="AY47" t="s">
-        <v>811</v>
+        <v>814</v>
       </c>
     </row>
-    <row r="48" spans="1:51">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -6995,10 +7031,10 @@
         <v>789</v>
       </c>
       <c r="AY48" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
-    <row r="49" spans="1:51">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -7047,8 +7083,11 @@
       <c r="AG49" t="s">
         <v>98</v>
       </c>
+      <c r="AY49" t="s">
+        <v>815</v>
+      </c>
     </row>
-    <row r="50" spans="1:51">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -7098,10 +7137,10 @@
         <v>790</v>
       </c>
       <c r="AY50" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
     </row>
-    <row r="51" spans="1:51">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -7151,7 +7190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:51">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -7237,7 +7276,7 @@
         <v>101</v>
       </c>
       <c r="AR52" s="2">
-        <v>85.40416666666667</v>
+        <v>85.404166666666669</v>
       </c>
       <c r="AT52" t="s">
         <v>767</v>
@@ -7246,7 +7285,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="53" spans="1:51">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -7305,7 +7344,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="54" spans="1:51">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -7334,7 +7373,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:51">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -7405,10 +7444,10 @@
         <v>104</v>
       </c>
       <c r="AY55" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
     </row>
-    <row r="56" spans="1:51">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -7437,10 +7476,10 @@
         <v>105</v>
       </c>
       <c r="AY56" t="s">
-        <v>814</v>
+        <v>818</v>
       </c>
     </row>
-    <row r="57" spans="1:51">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -7520,7 +7559,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="58" spans="1:51">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -7591,7 +7630,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:51">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -7665,10 +7704,10 @@
         <v>791</v>
       </c>
       <c r="AY59" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
     </row>
-    <row r="60" spans="1:51">
+    <row r="60" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -7724,7 +7763,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="61" spans="1:51">
+    <row r="61" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -7795,10 +7834,10 @@
         <v>792</v>
       </c>
       <c r="AY61" t="s">
-        <v>815</v>
+        <v>819</v>
       </c>
     </row>
-    <row r="62" spans="1:51">
+    <row r="62" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -7827,7 +7866,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:51">
+    <row r="63" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -7918,8 +7957,11 @@
       <c r="AT63">
         <v>2013</v>
       </c>
+      <c r="AY63" t="s">
+        <v>815</v>
+      </c>
     </row>
-    <row r="64" spans="1:51">
+    <row r="64" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>113</v>
       </c>
@@ -7993,10 +8035,10 @@
         <v>793</v>
       </c>
       <c r="AY64" t="s">
-        <v>816</v>
+        <v>820</v>
       </c>
     </row>
-    <row r="65" spans="1:51">
+    <row r="65" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>114</v>
       </c>
@@ -8085,7 +8127,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="66" spans="1:51">
+    <row r="66" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>115</v>
       </c>
@@ -8144,7 +8186,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:51">
+    <row r="67" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>116</v>
       </c>
@@ -8215,7 +8257,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="68" spans="1:51">
+    <row r="68" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>117</v>
       </c>
@@ -8337,7 +8379,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:51">
+    <row r="69" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>118</v>
       </c>
@@ -8420,7 +8462,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="70" spans="1:51">
+    <row r="70" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -8491,7 +8533,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="71" spans="1:51">
+    <row r="71" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>120</v>
       </c>
@@ -8520,7 +8562,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="1:51">
+    <row r="72" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -8579,7 +8621,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="73" spans="1:51">
+    <row r="73" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>122</v>
       </c>
@@ -8608,7 +8650,7 @@
         <v>122</v>
       </c>
       <c r="AY73" t="s">
-        <v>817</v>
+        <v>821</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Move everything from playground to main file
</commit_message>
<xml_diff>
--- a/Updated Zone 1 Activity Playground.xlsx
+++ b/Updated Zone 1 Activity Playground.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/munenekariuki/Downloads/GitHub/SPS-Report-Automation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{816FB89B-AA05-2E44-BA06-59290344926D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -2451,11 +2457,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2519,13 +2525,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2563,7 +2577,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -2597,6 +2611,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2631,9 +2646,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2806,14 +2822,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AV30" sqref="AV30"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="48" max="48" width="61.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2968,7 +2989,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
+    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -3084,7 +3105,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -3185,7 +3206,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -3268,7 +3289,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -3357,7 +3378,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -3446,7 +3467,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>56</v>
       </c>
@@ -3568,7 +3589,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>57</v>
       </c>
@@ -3684,7 +3705,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>58</v>
       </c>
@@ -3782,7 +3803,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -3886,7 +3907,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="11" spans="1:51">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>60</v>
       </c>
@@ -3975,7 +3996,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="12" spans="1:51">
+    <row r="12" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>61</v>
       </c>
@@ -4082,7 +4103,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="13" spans="1:51">
+    <row r="13" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>62</v>
       </c>
@@ -4180,7 +4201,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="14" spans="1:51">
+    <row r="14" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -4296,7 +4317,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="15" spans="1:51">
+    <row r="15" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -4427,7 +4448,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="16" spans="1:51">
+    <row r="16" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>65</v>
       </c>
@@ -4516,7 +4537,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="17" spans="1:51">
+    <row r="17" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>66</v>
       </c>
@@ -4629,7 +4650,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="18" spans="1:51">
+    <row r="18" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -4724,7 +4745,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="19" spans="1:51">
+    <row r="19" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>68</v>
       </c>
@@ -4840,7 +4861,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="20" spans="1:51">
+    <row r="20" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -4953,7 +4974,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="21" spans="1:51">
+    <row r="21" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>70</v>
       </c>
@@ -5057,7 +5078,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="22" spans="1:51">
+    <row r="22" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>71</v>
       </c>
@@ -5113,7 +5134,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="23" spans="1:51">
+    <row r="23" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -5226,7 +5247,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="24" spans="1:51">
+    <row r="24" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>73</v>
       </c>
@@ -5315,7 +5336,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="25" spans="1:51">
+    <row r="25" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -5422,7 +5443,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="26" spans="1:51">
+    <row r="26" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>75</v>
       </c>
@@ -5514,7 +5535,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="27" spans="1:51">
+    <row r="27" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>76</v>
       </c>
@@ -5615,7 +5636,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="28" spans="1:51">
+    <row r="28" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>77</v>
       </c>
@@ -5689,7 +5710,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="29" spans="1:51">
+    <row r="29" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>78</v>
       </c>
@@ -5784,7 +5805,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="30" spans="1:51">
+    <row r="30" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -5816,7 +5837,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="31" spans="1:51">
+    <row r="31" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -5848,7 +5869,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="32" spans="1:51">
+    <row r="32" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -5910,7 +5931,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="33" spans="1:51">
+    <row r="33" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>82</v>
       </c>
@@ -5936,7 +5957,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="34" spans="1:51">
+    <row r="34" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -5974,7 +5995,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="35" spans="1:51">
+    <row r="35" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>84</v>
       </c>
@@ -6048,7 +6069,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="36" spans="1:51">
+    <row r="36" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>85</v>
       </c>
@@ -6119,7 +6140,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="37" spans="1:51">
+    <row r="37" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>86</v>
       </c>
@@ -6148,7 +6169,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="38" spans="1:51">
+    <row r="38" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -6240,7 +6261,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="39" spans="1:51">
+    <row r="39" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>88</v>
       </c>
@@ -6329,7 +6350,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="40" spans="1:51">
+    <row r="40" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>89</v>
       </c>
@@ -6406,7 +6427,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="41" spans="1:51">
+    <row r="41" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>90</v>
       </c>
@@ -6495,7 +6516,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="42" spans="1:51">
+    <row r="42" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -6584,7 +6605,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="43" spans="1:51">
+    <row r="43" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>92</v>
       </c>
@@ -6655,7 +6676,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="44" spans="1:51">
+    <row r="44" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>93</v>
       </c>
@@ -6684,7 +6705,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="45" spans="1:51">
+    <row r="45" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>94</v>
       </c>
@@ -6716,7 +6737,7 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="46" spans="1:51">
+    <row r="46" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>95</v>
       </c>
@@ -6748,7 +6769,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="47" spans="1:51">
+    <row r="47" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>96</v>
       </c>
@@ -6843,7 +6864,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="48" spans="1:51">
+    <row r="48" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -6926,7 +6947,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="49" spans="1:51">
+    <row r="49" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>98</v>
       </c>
@@ -6970,7 +6991,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:51">
+    <row r="50" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>99</v>
       </c>
@@ -7023,7 +7044,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="51" spans="1:51">
+    <row r="51" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>100</v>
       </c>
@@ -7073,7 +7094,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:51">
+    <row r="52" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>101</v>
       </c>
@@ -7159,7 +7180,7 @@
         <v>101</v>
       </c>
       <c r="AR52" s="2">
-        <v>85.40416666666667</v>
+        <v>85.404166666666669</v>
       </c>
       <c r="AT52" t="s">
         <v>747</v>
@@ -7168,7 +7189,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="53" spans="1:51">
+    <row r="53" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>102</v>
       </c>
@@ -7227,7 +7248,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="54" spans="1:51">
+    <row r="54" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>103</v>
       </c>
@@ -7256,7 +7277,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:51">
+    <row r="55" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>104</v>
       </c>
@@ -7330,7 +7351,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="56" spans="1:51">
+    <row r="56" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>105</v>
       </c>
@@ -7362,7 +7383,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="57" spans="1:51">
+    <row r="57" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>106</v>
       </c>
@@ -7442,7 +7463,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="58" spans="1:51">
+    <row r="58" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>107</v>
       </c>
@@ -7513,7 +7534,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:51">
+    <row r="59" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>108</v>
       </c>
@@ -7590,7 +7611,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="60" spans="1:51">
+    <row r="60" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>109</v>
       </c>
@@ -7646,7 +7667,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="61" spans="1:51">
+    <row r="61" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -7720,7 +7741,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="62" spans="1:51">
+    <row r="62" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>111</v>
       </c>
@@ -7749,7 +7770,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="63" spans="1:51">
+    <row r="63" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>112</v>
       </c>
@@ -7838,7 +7859,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="64" spans="1:51">
+    <row r="64" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>113</v>
       </c>
@@ -7915,7 +7936,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="65" spans="1:51">
+    <row r="65" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>114</v>
       </c>
@@ -8004,7 +8025,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="66" spans="1:51">
+    <row r="66" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>115</v>
       </c>
@@ -8063,7 +8084,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="67" spans="1:51">
+    <row r="67" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>116</v>
       </c>
@@ -8134,7 +8155,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="68" spans="1:51">
+    <row r="68" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>117</v>
       </c>
@@ -8256,7 +8277,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="69" spans="1:51">
+    <row r="69" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>118</v>
       </c>
@@ -8339,7 +8360,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="70" spans="1:51">
+    <row r="70" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>119</v>
       </c>
@@ -8410,7 +8431,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="71" spans="1:51">
+    <row r="71" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>120</v>
       </c>
@@ -8439,7 +8460,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="1:51">
+    <row r="72" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>121</v>
       </c>
@@ -8498,7 +8519,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="73" spans="1:51">
+    <row r="73" spans="1:51" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>122</v>
       </c>

</xml_diff>